<commit_message>
Revamp the OP codebase according to the new OP structure
</commit_message>
<xml_diff>
--- a/flask-server/ontobot/files/excel/4961e33b-29d3-47ad-89a2-34d04dfff39babc.xlsx
+++ b/flask-server/ontobot/files/excel/4961e33b-29d3-47ad-89a2-34d04dfff39babc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Ontobot\ontobot-app\flask-server\ontobot\files\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CF7DD6-A290-4B6A-9F21-04B241EFD328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38DACE4-B121-4200-A38B-9FE149401261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="Student" sheetId="5" r:id="rId5"/>
     <sheet name="Toxic Student" sheetId="6" r:id="rId6"/>
     <sheet name="Innocent Student" sheetId="7" r:id="rId7"/>
-    <sheet name="Toxic Female Student" sheetId="8" r:id="rId8"/>
-    <sheet name="Toxic Male Student" sheetId="9" r:id="rId9"/>
+    <sheet name="Toxic Male Student" sheetId="9" r:id="rId8"/>
+    <sheet name="Toxic Female Student" sheetId="8" r:id="rId9"/>
     <sheet name="Lecture" sheetId="10" r:id="rId10"/>
     <sheet name="Juinor Lecture" sheetId="11" r:id="rId11"/>
     <sheet name="Senior Lecture" sheetId="12" r:id="rId12"/>
@@ -497,9 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,9 +624,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,12 +995,44 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,36 +1056,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new error messages and warning messages
</commit_message>
<xml_diff>
--- a/flask-server/ontobot/files/excel/4961e33b-29d3-47ad-89a2-34d04dfff39babc.xlsx
+++ b/flask-server/ontobot/files/excel/4961e33b-29d3-47ad-89a2-34d04dfff39babc.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Ontobot\ontobot-app\flask-server\ontobot\files\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38DACE4-B121-4200-A38B-9FE149401261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -20,22 +14,22 @@
     <sheet name="Student" sheetId="5" r:id="rId5"/>
     <sheet name="Toxic Student" sheetId="6" r:id="rId6"/>
     <sheet name="Innocent Student" sheetId="7" r:id="rId7"/>
-    <sheet name="Toxic Male Student" sheetId="9" r:id="rId8"/>
-    <sheet name="Toxic Female Student" sheetId="8" r:id="rId9"/>
+    <sheet name="Toxic Female Student" sheetId="8" r:id="rId8"/>
+    <sheet name="Toxic Male Student" sheetId="9" r:id="rId9"/>
     <sheet name="Lecture" sheetId="10" r:id="rId10"/>
-    <sheet name="Juinor Lecture" sheetId="11" r:id="rId11"/>
+    <sheet name="Junior Lecture" sheetId="11" r:id="rId11"/>
     <sheet name="Senior Lecture" sheetId="12" r:id="rId12"/>
     <sheet name="Degree" sheetId="13" r:id="rId13"/>
     <sheet name="CS Degree" sheetId="14" r:id="rId14"/>
     <sheet name="IS Degree" sheetId="15" r:id="rId15"/>
     <sheet name="SE Degree" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
   <si>
     <t># Object Name</t>
   </si>
@@ -63,57 +57,12 @@
   <si>
     <t>Degree Name (string)</t>
   </si>
-  <si>
-    <t>IFS</t>
-  </si>
-  <si>
-    <t>International Financial System</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Ananda College</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>RC</t>
-  </si>
-  <si>
-    <t>Royal College</t>
-  </si>
-  <si>
-    <t>UOC</t>
-  </si>
-  <si>
-    <t>Colombo</t>
-  </si>
-  <si>
-    <t>YOJ</t>
-  </si>
-  <si>
-    <t>Jaffna</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>IS</t>
-  </si>
-  <si>
-    <t>Information Systems</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,14 +112,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -217,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,27 +190,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,24 +224,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,22 +399,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -520,24 +425,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1997</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -545,13 +439,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -565,7 +459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -573,13 +467,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,7 +487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -601,13 +495,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -621,21 +515,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -643,29 +537,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -673,13 +551,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -693,7 +571,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -701,13 +579,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -721,7 +599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -729,13 +607,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -749,23 +627,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -779,56 +657,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1890</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1880</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -839,35 +689,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1900</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -875,15 +703,15 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -903,7 +731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -911,13 +739,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -931,7 +759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -939,14 +767,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -963,7 +791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -971,14 +799,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -995,7 +823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1003,14 +831,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1027,22 +855,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>